<commit_message>
delete boxit & graphmaker
</commit_message>
<xml_diff>
--- a/config template.xlsx
+++ b/config template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t xml:space="preserve">* </t>
   </si>
@@ -281,6 +281,14 @@
   </si>
   <si>
     <t>Use Dropbox</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Use UTF8 if you include this in Unity</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1327,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1376,31 +1384,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>2</v>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>2</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -1416,28 +1427,19 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -1445,13 +1447,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
-        <v>10</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -1459,35 +1461,32 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <v>0.95</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>18</v>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -1495,37 +1494,46 @@
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>2</v>
+    <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -1533,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -1541,7 +1549,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -1549,12 +1557,15 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
@@ -1562,26 +1573,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="9" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -1589,51 +1591,51 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
       </c>
+      <c r="E29" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C31" s="3">
         <v>0.2</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="7" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
@@ -1641,10 +1643,13 @@
         <v>27</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
@@ -1652,13 +1657,10 @@
         <v>27</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="5">
-        <v>90</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>42</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
@@ -1666,40 +1668,40 @@
         <v>27</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="5">
+        <v>90</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="5">
-        <v>2</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1707,13 +1709,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1721,10 +1723,13 @@
         <v>27</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C41" s="4">
-        <v>-30</v>
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1732,13 +1737,10 @@
         <v>27</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>52</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1746,13 +1748,13 @@
         <v>27</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4">
         <v>1</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1760,13 +1762,13 @@
         <v>27</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1774,16 +1776,13 @@
         <v>27</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="4" t="b">
+        <v>55</v>
+      </c>
+      <c r="C45" s="4">
         <v>0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1791,10 +1790,16 @@
         <v>27</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="4">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="C46" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1802,16 +1807,10 @@
         <v>27</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="C47" s="4">
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1819,10 +1818,16 @@
         <v>27</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="4">
-        <v>90</v>
+        <v>60</v>
+      </c>
+      <c r="C48" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -1830,37 +1835,34 @@
         <v>27</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C50" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="10" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -1868,46 +1870,55 @@
         <v>27</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C53" s="8">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="8" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="C54" s="8">
         <v>0.5</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C56" s="8">
         <v>1</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
@@ -1916,52 +1927,57 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="8" t="s">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B59" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C58" t="b">
+      <c r="C59" t="b">
         <v>1</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>2</v>
       </c>
-      <c r="B60" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>75</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>77</v>
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>75</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <hyperlinks>
-    <hyperlink ref="B61" r:id="rId1" location="!/content/4096"/>
+    <hyperlink ref="B62" r:id="rId1" location="!/content/4096"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sample protocol & manual
</commit_message>
<xml_diff>
--- a/config template.xlsx
+++ b/config template.xlsx
@@ -14,27 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
   <si>
     <t xml:space="preserve">* </t>
   </si>
   <si>
-    <t>configuration file with default values</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
-    <t>common parameters</t>
-  </si>
-  <si>
     <t>Field Name は、読み込む際に用いるので、1列目は変更しないこと</t>
-  </si>
-  <si>
-    <t>lines that begin with "*" are regarded as comment, and will be ignored</t>
-  </si>
-  <si>
-    <t>* から始まる行はコメント行として無視する（コメント記号はscriptから変更可能）</t>
   </si>
   <si>
     <t>Field Name</t>
@@ -219,10 +207,6 @@
   </si>
   <si>
     <t>*</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>caution: Do not change field names!</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -268,27 +252,41 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
+    <t>Lines that begin with "*" are regarded as comment. These will be ignored.</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Configuration settings</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>caution: Do not change field names (column A)!</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>* から始まる行はコメント行として無視する</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
     <t>*</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>Dropbox (requires unity asset: boxit)</t>
+    <t>config.csv として、スマートデバイスのpersistentDataPathに移して使う</t>
+    <rPh sb="43" eb="44">
+      <t>ウツ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ツカ</t>
+    </rPh>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>https://www.assetstore.unity3d.com/jp/#!/content/4096</t>
+    <t>Modify parameters, rename the file as "config.csv", and move the file to persistentDataPath of the device</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>Use Dropbox</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Use UTF8 if you include this in Unity</t>
+    <t>(In Android devices, persistentDataPath is "/data/data/PoMLabProject.PoMLabApp/files")</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -296,7 +294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,15 +455,6 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="43">
     <fill>
@@ -824,7 +813,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -951,11 +940,8 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -989,11 +975,8 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - アクセント 1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - アクセント 2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - アクセント 3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1021,7 +1004,6 @@
     <cellStyle name="タイトル" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="チェック セル" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="どちらでもない" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="ハイパーリンク" xfId="42" builtinId="8"/>
     <cellStyle name="メモ" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="リンク セル" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="悪い" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1335,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1352,260 +1334,263 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>80</v>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2">
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2">
         <v>0.95</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -1613,51 +1598,51 @@
     </row>
     <row r="31" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C31" s="3">
         <v>0.2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C34" s="5">
         <v>0.1</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C35" s="5">
         <v>0.5</v>
@@ -1665,79 +1650,79 @@
     </row>
     <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C36" s="5">
         <v>90</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C37" s="5">
         <v>2</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40" s="4">
         <v>0.1</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C42" s="4">
         <v>-30</v>
@@ -1745,69 +1730,69 @@
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C43" s="4">
         <v>1</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C45" s="4">
         <v>0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C46" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C47" s="4">
         <v>90</v>
@@ -1815,27 +1800,27 @@
     </row>
     <row r="48" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C48" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C49" s="4">
         <v>90</v>
@@ -1843,10 +1828,10 @@
     </row>
     <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C50" s="4">
         <v>1</v>
@@ -1854,131 +1839,99 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C53" s="8">
         <v>1.5</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C54" s="8">
         <v>0.5</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C55" s="8">
         <v>0.5</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C56" s="8">
         <v>1</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
-  <hyperlinks>
-    <hyperlink ref="B62" r:id="rId1" location="!/content/4096"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>